<commit_message>
update mail and aproval
</commit_message>
<xml_diff>
--- a/DB.xlsx
+++ b/DB.xlsx
@@ -5,14 +5,16 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\daita\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\thezo\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="120" yWindow="100" windowWidth="23900" windowHeight="14540" tabRatio="728"/>
+    <workbookView xWindow="120" yWindow="100" windowWidth="23900" windowHeight="14540" tabRatio="728" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="member(sample)" sheetId="2" r:id="rId1"/>
+    <sheet name="approval" sheetId="3" r:id="rId2"/>
+    <sheet name="mail" sheetId="4" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'member(sample)'!$A$1:$Q$491</definedName>
@@ -9299,8 +9301,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q491"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H43" sqref="H43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="19.6640625" defaultRowHeight="17" x14ac:dyDescent="0.45"/>
@@ -33436,4 +33438,33 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
+  <sheetData/>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="X16" sqref="X16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
+  <sheetData/>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
add: 문서관리, 일정관리 파트 sequence생성문 추가, document sample data 추가
</commit_message>
<xml_diff>
--- a/DB.xlsx
+++ b/DB.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24131"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\thezo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\finalProject\thezo\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{502909F4-A3AA-4017-A5C7-52014D1065DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="108" windowWidth="23892" windowHeight="13740" tabRatio="728" firstSheet="4" activeTab="11"/>
+    <workbookView xWindow="5712" yWindow="348" windowWidth="17004" windowHeight="10404" tabRatio="728" firstSheet="10" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="member(sample)" sheetId="2" r:id="rId1"/>
@@ -25,6 +26,7 @@
     <sheet name="Jaewon_message" sheetId="12" r:id="rId11"/>
     <sheet name="Jaewon_msg_report" sheetId="13" r:id="rId12"/>
     <sheet name="Jaewon_admin_log" sheetId="14" r:id="rId13"/>
+    <sheet name="Sunyoung_document" sheetId="15" r:id="rId14"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'member(sample)'!$A$1:$Q$491</definedName>
@@ -35,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1344" uniqueCount="638">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1412" uniqueCount="666">
   <si>
     <t xml:space="preserve">	서울특별시송파구올림픽로 99(잠실동, 잠실엘스)</t>
   </si>
@@ -2200,12 +2202,124 @@
   <si>
     <t>기초적인 모든 세팅과 회사 설정 등등</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DOC_NO</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>DOC_WRITER</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>DOC_CONTENT</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>DOC_CATEGORY</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>CREATE_DATE</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>CHANGE_NAME</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>STATUS</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>공문 발송 양식입니다.</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>공용</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>회의록 양식 입니다. 업무에 참고바랍니다.</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>시말서 입니다.</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>2021년 프로젝트 보고서 양식 입니다.</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>발주서</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>기본 계약서</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>기본 계약서(내용 추가)</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>출장 보고서 양식</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>사유서 양식</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>업무일지 양식입니다. 참고하여 작성 바랍니다.</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>회사소개서 양식</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>교육보고서 양식</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>근로계약서</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>품의서</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>문서 발송 대장</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>기본 보고서 양식 입니다.</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>저희 회사 마크입니다~~~</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>사업자 등록증</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>수습사원 평가서 입니다 !!</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>개정된 회의록 양식입니다. 업무에 참고바랍니다.</t>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -2410,7 +2524,7 @@
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
-    <cellStyle name="표준 2" xfId="2"/>
+    <cellStyle name="표준 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
     <cellStyle name="하이퍼링크" xfId="1" builtinId="8"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2502,6 +2616,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -2537,6 +2668,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -2712,7 +2860,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Y492"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
@@ -14711,10 +14859,10 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="G2" r:id="rId1"/>
-    <hyperlink ref="G3" r:id="rId2"/>
-    <hyperlink ref="G46:G86" r:id="rId3" display="user01@thezo.com"/>
-    <hyperlink ref="G4:G73" r:id="rId4" display="user01@thezo.com"/>
+    <hyperlink ref="G2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="G3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="G46:G86" r:id="rId3" display="user01@thezo.com" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="G4:G73" r:id="rId4" display="user01@thezo.com" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" r:id="rId5"/>
@@ -14722,11 +14870,11 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -14831,7 +14979,7 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:L19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -15583,10 +15731,10 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:L3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
@@ -15721,7 +15869,7 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -15798,8 +15946,501 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62E9B575-B50C-404F-BDA9-D0FC06A60F26}">
+  <dimension ref="A1:H21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="1" max="1" width="8.296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.69921875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="41.09765625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.59765625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.296875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.09765625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.296875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A1" s="4" t="s">
+        <v>638</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>639</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>640</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>641</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>642</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>228</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>643</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>644</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A2" s="4">
+        <v>1</v>
+      </c>
+      <c r="B2" s="4">
+        <v>2</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>645</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>646</v>
+      </c>
+      <c r="E2" s="8">
+        <v>44256</v>
+      </c>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A3" s="4">
+        <v>2</v>
+      </c>
+      <c r="B3" s="4">
+        <v>5</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>647</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>646</v>
+      </c>
+      <c r="E3" s="8">
+        <v>44257</v>
+      </c>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A4" s="4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="4">
+        <v>9</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>648</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>646</v>
+      </c>
+      <c r="E4" s="8">
+        <v>44258</v>
+      </c>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A5" s="4">
+        <v>4</v>
+      </c>
+      <c r="B5" s="4">
+        <v>8</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>649</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>646</v>
+      </c>
+      <c r="E5" s="8">
+        <v>44259</v>
+      </c>
+      <c r="F5" s="4"/>
+      <c r="G5" s="4"/>
+      <c r="H5" s="4" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A6" s="4">
+        <v>5</v>
+      </c>
+      <c r="B6" s="4">
+        <v>4</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>650</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>646</v>
+      </c>
+      <c r="E6" s="8">
+        <v>44260</v>
+      </c>
+      <c r="F6" s="4"/>
+      <c r="G6" s="4"/>
+      <c r="H6" s="4" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A7" s="4">
+        <v>6</v>
+      </c>
+      <c r="B7" s="4">
+        <v>6</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>651</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>646</v>
+      </c>
+      <c r="E7" s="8">
+        <v>44261</v>
+      </c>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
+      <c r="H7" s="4" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A8" s="4">
+        <v>7</v>
+      </c>
+      <c r="B8" s="4">
+        <v>6</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>652</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>646</v>
+      </c>
+      <c r="E8" s="8">
+        <v>44262</v>
+      </c>
+      <c r="F8" s="4"/>
+      <c r="G8" s="4"/>
+      <c r="H8" s="4" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A9" s="4">
+        <v>8</v>
+      </c>
+      <c r="B9" s="4">
+        <v>6</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>653</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>646</v>
+      </c>
+      <c r="E9" s="8">
+        <v>44263</v>
+      </c>
+      <c r="F9" s="4"/>
+      <c r="G9" s="4"/>
+      <c r="H9" s="4" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A10" s="4">
+        <v>9</v>
+      </c>
+      <c r="B10" s="4">
+        <v>7</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>654</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>646</v>
+      </c>
+      <c r="E10" s="8">
+        <v>44264</v>
+      </c>
+      <c r="F10" s="4"/>
+      <c r="G10" s="4"/>
+      <c r="H10" s="4" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A11" s="4">
+        <v>10</v>
+      </c>
+      <c r="B11" s="4">
+        <v>9</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>655</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>646</v>
+      </c>
+      <c r="E11" s="8">
+        <v>44265</v>
+      </c>
+      <c r="F11" s="4"/>
+      <c r="G11" s="4"/>
+      <c r="H11" s="4" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A12" s="4">
+        <v>11</v>
+      </c>
+      <c r="B12" s="4">
+        <v>3</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>656</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>646</v>
+      </c>
+      <c r="E12" s="8">
+        <v>44266</v>
+      </c>
+      <c r="F12" s="4"/>
+      <c r="G12" s="4"/>
+      <c r="H12" s="4" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A13" s="4">
+        <v>12</v>
+      </c>
+      <c r="B13" s="4">
+        <v>3</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>657</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>646</v>
+      </c>
+      <c r="E13" s="8">
+        <v>44267</v>
+      </c>
+      <c r="F13" s="4"/>
+      <c r="G13" s="4"/>
+      <c r="H13" s="4" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A14" s="4">
+        <v>13</v>
+      </c>
+      <c r="B14" s="4">
+        <v>3</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>658</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>646</v>
+      </c>
+      <c r="E14" s="8">
+        <v>44268</v>
+      </c>
+      <c r="F14" s="4"/>
+      <c r="G14" s="4"/>
+      <c r="H14" s="4" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A15" s="4">
+        <v>14</v>
+      </c>
+      <c r="B15" s="4">
+        <v>7</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>659</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>646</v>
+      </c>
+      <c r="E15" s="8">
+        <v>44269</v>
+      </c>
+      <c r="F15" s="4"/>
+      <c r="G15" s="4"/>
+      <c r="H15" s="4" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A16" s="4">
+        <v>15</v>
+      </c>
+      <c r="B16" s="4">
+        <v>5</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>660</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>646</v>
+      </c>
+      <c r="E16" s="8">
+        <v>44270</v>
+      </c>
+      <c r="F16" s="4"/>
+      <c r="G16" s="4"/>
+      <c r="H16" s="4" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A17" s="4">
+        <v>16</v>
+      </c>
+      <c r="B17" s="4">
+        <v>10</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>661</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>646</v>
+      </c>
+      <c r="E17" s="8">
+        <v>44271</v>
+      </c>
+      <c r="F17" s="4"/>
+      <c r="G17" s="4"/>
+      <c r="H17" s="4" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A18" s="4">
+        <v>17</v>
+      </c>
+      <c r="B18" s="4">
+        <v>5</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>662</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>646</v>
+      </c>
+      <c r="E18" s="8">
+        <v>44272</v>
+      </c>
+      <c r="F18" s="4"/>
+      <c r="G18" s="4"/>
+      <c r="H18" s="4" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A19" s="4">
+        <v>18</v>
+      </c>
+      <c r="B19" s="4">
+        <v>5</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>663</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>646</v>
+      </c>
+      <c r="E19" s="8">
+        <v>44273</v>
+      </c>
+      <c r="F19" s="4"/>
+      <c r="G19" s="4"/>
+      <c r="H19" s="4" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A20" s="4">
+        <v>19</v>
+      </c>
+      <c r="B20" s="4">
+        <v>5</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>664</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>646</v>
+      </c>
+      <c r="E20" s="8">
+        <v>44274</v>
+      </c>
+      <c r="F20" s="4"/>
+      <c r="G20" s="4"/>
+      <c r="H20" s="4" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A21" s="4">
+        <v>20</v>
+      </c>
+      <c r="B21" s="4">
+        <v>4</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>665</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>646</v>
+      </c>
+      <c r="E21" s="8">
+        <v>44275</v>
+      </c>
+      <c r="F21" s="4"/>
+      <c r="G21" s="4"/>
+      <c r="H21" s="4" t="s">
+        <v>242</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -15813,7 +16454,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -15828,7 +16469,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -16004,7 +16645,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -16190,7 +16831,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -16428,7 +17069,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:G32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -17035,7 +17676,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:I17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -17460,7 +18101,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>

<commit_message>
add : sample data 추가
-  report sample data 추가
</commit_message>
<xml_diff>
--- a/DB.xlsx
+++ b/DB.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="5715" yWindow="345" windowWidth="17010" windowHeight="10410" tabRatio="728" firstSheet="9" activeTab="16"/>
+    <workbookView xWindow="5715" yWindow="345" windowWidth="17010" windowHeight="10410" tabRatio="728" firstSheet="9" activeTab="17"/>
   </bookViews>
   <sheets>
     <sheet name="member(sample)" sheetId="2" r:id="rId1"/>
@@ -21,9 +21,10 @@
     <sheet name="Jaewon_msg_report" sheetId="13" r:id="rId12"/>
     <sheet name="Jaewon_admin_log" sheetId="14" r:id="rId13"/>
     <sheet name="Sunyoung_document" sheetId="15" r:id="rId14"/>
-    <sheet name="Lsk_board" sheetId="16" r:id="rId15"/>
-    <sheet name="Lsk_market" sheetId="17" r:id="rId16"/>
-    <sheet name="Lsk_reply" sheetId="18" r:id="rId17"/>
+    <sheet name="SK_board" sheetId="16" r:id="rId15"/>
+    <sheet name="SK_market" sheetId="17" r:id="rId16"/>
+    <sheet name="SK_reply" sheetId="18" r:id="rId17"/>
+    <sheet name="SK_report" sheetId="19" r:id="rId18"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'member(sample)'!$A$1:$Q$491</definedName>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1805" uniqueCount="816">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1935" uniqueCount="835">
   <si>
     <t xml:space="preserve">	서울특별시송파구올림픽로 99(잠실동, 잠실엘스)</t>
   </si>
@@ -2837,6 +2838,73 @@
   </si>
   <si>
     <t>디자인 별론데 양심없음?</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>RP_CODE</t>
+  </si>
+  <si>
+    <t>RP_ID</t>
+  </si>
+  <si>
+    <t>RP_DATE</t>
+  </si>
+  <si>
+    <t>BOARD_TYPE</t>
+  </si>
+  <si>
+    <t>RP_TYPE</t>
+  </si>
+  <si>
+    <t>RP_NO</t>
+  </si>
+  <si>
+    <t>RP_SECTION</t>
+  </si>
+  <si>
+    <t>RP_CONTENT</t>
+  </si>
+  <si>
+    <t>HANDLING_DATE</t>
+  </si>
+  <si>
+    <t>user40</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>욕설/비방</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">욕설 신고 </t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Y</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>도배/스팸</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>도배 신고</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Y</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>user40</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>욕설/비방</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">욕설 신고 </t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
 </sst>
@@ -19491,7 +19559,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
@@ -19640,6 +19708,1027 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J31"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O12" sqref="O12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="9" style="6"/>
+    <col min="2" max="2" width="12.125" style="6" customWidth="1"/>
+    <col min="3" max="3" width="11.125" style="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14" style="6" customWidth="1"/>
+    <col min="5" max="5" width="11.75" style="6" customWidth="1"/>
+    <col min="6" max="6" width="9" style="6"/>
+    <col min="7" max="7" width="13.25" style="6" customWidth="1"/>
+    <col min="8" max="8" width="13.875" style="6" customWidth="1"/>
+    <col min="9" max="9" width="16" style="6" customWidth="1"/>
+    <col min="10" max="16384" width="9" style="6"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A1" s="6" t="s">
+        <v>816</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>817</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>818</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>819</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>820</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>821</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>822</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>823</v>
+      </c>
+      <c r="I1" s="6" t="s">
+        <v>824</v>
+      </c>
+      <c r="J1" s="6" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A2" s="6">
+        <v>1</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>825</v>
+      </c>
+      <c r="C2" s="28">
+        <v>44256</v>
+      </c>
+      <c r="D2" s="6">
+        <v>1</v>
+      </c>
+      <c r="E2" s="6">
+        <v>1</v>
+      </c>
+      <c r="F2" s="6">
+        <v>31</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>826</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>827</v>
+      </c>
+      <c r="I2" s="28">
+        <v>44256</v>
+      </c>
+      <c r="J2" s="6" t="s">
+        <v>828</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A3" s="6">
+        <v>2</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>412</v>
+      </c>
+      <c r="C3" s="28">
+        <v>44256</v>
+      </c>
+      <c r="D3" s="6">
+        <v>1</v>
+      </c>
+      <c r="E3" s="6">
+        <v>1</v>
+      </c>
+      <c r="F3" s="6">
+        <v>31</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>826</v>
+      </c>
+      <c r="H3" s="6" t="s">
+        <v>827</v>
+      </c>
+      <c r="I3" s="28">
+        <v>44256</v>
+      </c>
+      <c r="J3" s="6" t="s">
+        <v>828</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A4" s="6">
+        <v>3</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>415</v>
+      </c>
+      <c r="C4" s="28">
+        <v>44256</v>
+      </c>
+      <c r="D4" s="6">
+        <v>1</v>
+      </c>
+      <c r="E4" s="6">
+        <v>1</v>
+      </c>
+      <c r="F4" s="6">
+        <v>31</v>
+      </c>
+      <c r="G4" s="6" t="s">
+        <v>826</v>
+      </c>
+      <c r="H4" s="6" t="s">
+        <v>827</v>
+      </c>
+      <c r="I4" s="28">
+        <v>44256</v>
+      </c>
+      <c r="J4" s="6" t="s">
+        <v>828</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A5" s="6">
+        <v>4</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>418</v>
+      </c>
+      <c r="C5" s="28">
+        <v>44256</v>
+      </c>
+      <c r="D5" s="6">
+        <v>1</v>
+      </c>
+      <c r="E5" s="6">
+        <v>1</v>
+      </c>
+      <c r="F5" s="6">
+        <v>31</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>826</v>
+      </c>
+      <c r="H5" s="6" t="s">
+        <v>827</v>
+      </c>
+      <c r="I5" s="28">
+        <v>44256</v>
+      </c>
+      <c r="J5" s="6" t="s">
+        <v>828</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A6" s="6">
+        <v>5</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>421</v>
+      </c>
+      <c r="C6" s="28">
+        <v>44256</v>
+      </c>
+      <c r="D6" s="6">
+        <v>1</v>
+      </c>
+      <c r="E6" s="6">
+        <v>1</v>
+      </c>
+      <c r="F6" s="6">
+        <v>31</v>
+      </c>
+      <c r="G6" s="6" t="s">
+        <v>826</v>
+      </c>
+      <c r="H6" s="6" t="s">
+        <v>827</v>
+      </c>
+      <c r="I6" s="28">
+        <v>44256</v>
+      </c>
+      <c r="J6" s="6" t="s">
+        <v>828</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A7" s="6">
+        <v>6</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>424</v>
+      </c>
+      <c r="C7" s="28">
+        <v>44257</v>
+      </c>
+      <c r="D7" s="6">
+        <v>1</v>
+      </c>
+      <c r="E7" s="6">
+        <v>1</v>
+      </c>
+      <c r="F7" s="6">
+        <v>31</v>
+      </c>
+      <c r="G7" s="6" t="s">
+        <v>826</v>
+      </c>
+      <c r="H7" s="6" t="s">
+        <v>827</v>
+      </c>
+      <c r="I7" s="28">
+        <v>44257</v>
+      </c>
+      <c r="J7" s="6" t="s">
+        <v>828</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A8" s="6">
+        <v>7</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>427</v>
+      </c>
+      <c r="C8" s="28">
+        <v>44257</v>
+      </c>
+      <c r="D8" s="6">
+        <v>1</v>
+      </c>
+      <c r="E8" s="6">
+        <v>1</v>
+      </c>
+      <c r="F8" s="6">
+        <v>31</v>
+      </c>
+      <c r="G8" s="6" t="s">
+        <v>826</v>
+      </c>
+      <c r="H8" s="6" t="s">
+        <v>827</v>
+      </c>
+      <c r="I8" s="28">
+        <v>44257</v>
+      </c>
+      <c r="J8" s="6" t="s">
+        <v>828</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A9" s="6">
+        <v>8</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>430</v>
+      </c>
+      <c r="C9" s="28">
+        <v>44257</v>
+      </c>
+      <c r="D9" s="6">
+        <v>1</v>
+      </c>
+      <c r="E9" s="6">
+        <v>1</v>
+      </c>
+      <c r="F9" s="6">
+        <v>31</v>
+      </c>
+      <c r="G9" s="6" t="s">
+        <v>826</v>
+      </c>
+      <c r="H9" s="6" t="s">
+        <v>827</v>
+      </c>
+      <c r="I9" s="28">
+        <v>44257</v>
+      </c>
+      <c r="J9" s="6" t="s">
+        <v>828</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A10" s="6">
+        <v>9</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>433</v>
+      </c>
+      <c r="C10" s="28">
+        <v>44257</v>
+      </c>
+      <c r="D10" s="6">
+        <v>1</v>
+      </c>
+      <c r="E10" s="6">
+        <v>1</v>
+      </c>
+      <c r="F10" s="6">
+        <v>31</v>
+      </c>
+      <c r="G10" s="6" t="s">
+        <v>826</v>
+      </c>
+      <c r="H10" s="6" t="s">
+        <v>827</v>
+      </c>
+      <c r="I10" s="28">
+        <v>44257</v>
+      </c>
+      <c r="J10" s="6" t="s">
+        <v>828</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A11" s="6">
+        <v>10</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>436</v>
+      </c>
+      <c r="C11" s="28">
+        <v>44257</v>
+      </c>
+      <c r="D11" s="6">
+        <v>1</v>
+      </c>
+      <c r="E11" s="6">
+        <v>1</v>
+      </c>
+      <c r="F11" s="6">
+        <v>31</v>
+      </c>
+      <c r="G11" s="6" t="s">
+        <v>826</v>
+      </c>
+      <c r="H11" s="6" t="s">
+        <v>827</v>
+      </c>
+      <c r="I11" s="28">
+        <v>44257</v>
+      </c>
+      <c r="J11" s="6" t="s">
+        <v>828</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A12" s="6">
+        <v>11</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>825</v>
+      </c>
+      <c r="C12" s="28">
+        <v>44257</v>
+      </c>
+      <c r="D12" s="6">
+        <v>1</v>
+      </c>
+      <c r="E12" s="6">
+        <v>1</v>
+      </c>
+      <c r="F12" s="6">
+        <v>31</v>
+      </c>
+      <c r="G12" s="6" t="s">
+        <v>826</v>
+      </c>
+      <c r="H12" s="6" t="s">
+        <v>827</v>
+      </c>
+      <c r="I12" s="28">
+        <v>44257</v>
+      </c>
+      <c r="J12" s="6" t="s">
+        <v>828</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A13" s="6">
+        <v>12</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>412</v>
+      </c>
+      <c r="C13" s="28">
+        <v>44258</v>
+      </c>
+      <c r="D13" s="6">
+        <v>1</v>
+      </c>
+      <c r="E13" s="6">
+        <v>1</v>
+      </c>
+      <c r="F13" s="6">
+        <v>32</v>
+      </c>
+      <c r="G13" s="6" t="s">
+        <v>829</v>
+      </c>
+      <c r="H13" s="6" t="s">
+        <v>830</v>
+      </c>
+      <c r="I13" s="28">
+        <v>44258</v>
+      </c>
+      <c r="J13" s="6" t="s">
+        <v>831</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A14" s="6">
+        <v>13</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>415</v>
+      </c>
+      <c r="C14" s="28">
+        <v>44258</v>
+      </c>
+      <c r="D14" s="6">
+        <v>1</v>
+      </c>
+      <c r="E14" s="6">
+        <v>1</v>
+      </c>
+      <c r="F14" s="6">
+        <v>32</v>
+      </c>
+      <c r="G14" s="6" t="s">
+        <v>829</v>
+      </c>
+      <c r="H14" s="6" t="s">
+        <v>830</v>
+      </c>
+      <c r="I14" s="28">
+        <v>44258</v>
+      </c>
+      <c r="J14" s="6" t="s">
+        <v>831</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A15" s="6">
+        <v>14</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>418</v>
+      </c>
+      <c r="C15" s="28">
+        <v>44258</v>
+      </c>
+      <c r="D15" s="6">
+        <v>1</v>
+      </c>
+      <c r="E15" s="6">
+        <v>1</v>
+      </c>
+      <c r="F15" s="6">
+        <v>32</v>
+      </c>
+      <c r="G15" s="6" t="s">
+        <v>829</v>
+      </c>
+      <c r="H15" s="6" t="s">
+        <v>830</v>
+      </c>
+      <c r="I15" s="28">
+        <v>44258</v>
+      </c>
+      <c r="J15" s="6" t="s">
+        <v>831</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A16" s="6">
+        <v>15</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>421</v>
+      </c>
+      <c r="C16" s="28">
+        <v>44258</v>
+      </c>
+      <c r="D16" s="6">
+        <v>1</v>
+      </c>
+      <c r="E16" s="6">
+        <v>1</v>
+      </c>
+      <c r="F16" s="6">
+        <v>32</v>
+      </c>
+      <c r="G16" s="6" t="s">
+        <v>829</v>
+      </c>
+      <c r="H16" s="6" t="s">
+        <v>830</v>
+      </c>
+      <c r="I16" s="28">
+        <v>44258</v>
+      </c>
+      <c r="J16" s="6" t="s">
+        <v>831</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A17" s="6">
+        <v>16</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>424</v>
+      </c>
+      <c r="C17" s="28">
+        <v>44258</v>
+      </c>
+      <c r="D17" s="6">
+        <v>1</v>
+      </c>
+      <c r="E17" s="6">
+        <v>1</v>
+      </c>
+      <c r="F17" s="6">
+        <v>32</v>
+      </c>
+      <c r="G17" s="6" t="s">
+        <v>829</v>
+      </c>
+      <c r="H17" s="6" t="s">
+        <v>830</v>
+      </c>
+      <c r="I17" s="28">
+        <v>44258</v>
+      </c>
+      <c r="J17" s="6" t="s">
+        <v>831</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A18" s="6">
+        <v>17</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>427</v>
+      </c>
+      <c r="C18" s="28">
+        <v>44258</v>
+      </c>
+      <c r="D18" s="6">
+        <v>1</v>
+      </c>
+      <c r="E18" s="6">
+        <v>1</v>
+      </c>
+      <c r="F18" s="6">
+        <v>32</v>
+      </c>
+      <c r="G18" s="6" t="s">
+        <v>829</v>
+      </c>
+      <c r="H18" s="6" t="s">
+        <v>830</v>
+      </c>
+      <c r="I18" s="28">
+        <v>44258</v>
+      </c>
+      <c r="J18" s="6" t="s">
+        <v>831</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A19" s="6">
+        <v>18</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>430</v>
+      </c>
+      <c r="C19" s="28">
+        <v>44258</v>
+      </c>
+      <c r="D19" s="6">
+        <v>1</v>
+      </c>
+      <c r="E19" s="6">
+        <v>1</v>
+      </c>
+      <c r="F19" s="6">
+        <v>32</v>
+      </c>
+      <c r="G19" s="6" t="s">
+        <v>829</v>
+      </c>
+      <c r="H19" s="6" t="s">
+        <v>830</v>
+      </c>
+      <c r="I19" s="28">
+        <v>44258</v>
+      </c>
+      <c r="J19" s="6" t="s">
+        <v>831</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A20" s="6">
+        <v>19</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>433</v>
+      </c>
+      <c r="C20" s="28">
+        <v>44258</v>
+      </c>
+      <c r="D20" s="6">
+        <v>1</v>
+      </c>
+      <c r="E20" s="6">
+        <v>1</v>
+      </c>
+      <c r="F20" s="6">
+        <v>32</v>
+      </c>
+      <c r="G20" s="6" t="s">
+        <v>829</v>
+      </c>
+      <c r="H20" s="6" t="s">
+        <v>830</v>
+      </c>
+      <c r="I20" s="28">
+        <v>44258</v>
+      </c>
+      <c r="J20" s="6" t="s">
+        <v>831</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A21" s="6">
+        <v>20</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>436</v>
+      </c>
+      <c r="C21" s="28">
+        <v>44258</v>
+      </c>
+      <c r="D21" s="6">
+        <v>1</v>
+      </c>
+      <c r="E21" s="6">
+        <v>1</v>
+      </c>
+      <c r="F21" s="6">
+        <v>32</v>
+      </c>
+      <c r="G21" s="6" t="s">
+        <v>829</v>
+      </c>
+      <c r="H21" s="6" t="s">
+        <v>830</v>
+      </c>
+      <c r="I21" s="28">
+        <v>44258</v>
+      </c>
+      <c r="J21" s="6" t="s">
+        <v>831</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A22" s="6">
+        <v>21</v>
+      </c>
+      <c r="B22" s="6" t="s">
+        <v>832</v>
+      </c>
+      <c r="C22" s="28">
+        <v>44265</v>
+      </c>
+      <c r="D22" s="6">
+        <v>1</v>
+      </c>
+      <c r="E22" s="6">
+        <v>1</v>
+      </c>
+      <c r="F22" s="6">
+        <v>40</v>
+      </c>
+      <c r="G22" s="6" t="s">
+        <v>833</v>
+      </c>
+      <c r="H22" s="6" t="s">
+        <v>834</v>
+      </c>
+      <c r="I22" s="28">
+        <v>44265</v>
+      </c>
+      <c r="J22" s="6" t="s">
+        <v>831</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A23" s="6">
+        <v>22</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>412</v>
+      </c>
+      <c r="C23" s="28">
+        <v>44266</v>
+      </c>
+      <c r="D23" s="6">
+        <v>1</v>
+      </c>
+      <c r="E23" s="6">
+        <v>1</v>
+      </c>
+      <c r="F23" s="6">
+        <v>40</v>
+      </c>
+      <c r="G23" s="6" t="s">
+        <v>833</v>
+      </c>
+      <c r="H23" s="6" t="s">
+        <v>834</v>
+      </c>
+      <c r="I23" s="28">
+        <v>44266</v>
+      </c>
+      <c r="J23" s="6" t="s">
+        <v>831</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A24" s="6">
+        <v>23</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>415</v>
+      </c>
+      <c r="C24" s="28">
+        <v>44267</v>
+      </c>
+      <c r="D24" s="6">
+        <v>1</v>
+      </c>
+      <c r="E24" s="6">
+        <v>1</v>
+      </c>
+      <c r="F24" s="6">
+        <v>40</v>
+      </c>
+      <c r="G24" s="6" t="s">
+        <v>833</v>
+      </c>
+      <c r="H24" s="6" t="s">
+        <v>834</v>
+      </c>
+      <c r="I24" s="28">
+        <v>44267</v>
+      </c>
+      <c r="J24" s="6" t="s">
+        <v>831</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A25" s="6">
+        <v>24</v>
+      </c>
+      <c r="B25" s="6" t="s">
+        <v>418</v>
+      </c>
+      <c r="C25" s="28">
+        <v>44268</v>
+      </c>
+      <c r="D25" s="6">
+        <v>1</v>
+      </c>
+      <c r="E25" s="6">
+        <v>1</v>
+      </c>
+      <c r="F25" s="6">
+        <v>40</v>
+      </c>
+      <c r="G25" s="6" t="s">
+        <v>833</v>
+      </c>
+      <c r="H25" s="6" t="s">
+        <v>834</v>
+      </c>
+      <c r="I25" s="28">
+        <v>44268</v>
+      </c>
+      <c r="J25" s="6" t="s">
+        <v>831</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A26" s="6">
+        <v>25</v>
+      </c>
+      <c r="B26" s="6" t="s">
+        <v>421</v>
+      </c>
+      <c r="C26" s="28">
+        <v>44269</v>
+      </c>
+      <c r="D26" s="6">
+        <v>1</v>
+      </c>
+      <c r="E26" s="6">
+        <v>1</v>
+      </c>
+      <c r="F26" s="6">
+        <v>40</v>
+      </c>
+      <c r="G26" s="6" t="s">
+        <v>833</v>
+      </c>
+      <c r="H26" s="6" t="s">
+        <v>834</v>
+      </c>
+      <c r="I26" s="28">
+        <v>44269</v>
+      </c>
+      <c r="J26" s="6" t="s">
+        <v>831</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A27" s="6">
+        <v>26</v>
+      </c>
+      <c r="B27" s="6" t="s">
+        <v>424</v>
+      </c>
+      <c r="C27" s="28">
+        <v>44270</v>
+      </c>
+      <c r="D27" s="6">
+        <v>1</v>
+      </c>
+      <c r="E27" s="6">
+        <v>1</v>
+      </c>
+      <c r="F27" s="6">
+        <v>40</v>
+      </c>
+      <c r="G27" s="6" t="s">
+        <v>833</v>
+      </c>
+      <c r="H27" s="6" t="s">
+        <v>834</v>
+      </c>
+      <c r="I27" s="28">
+        <v>44270</v>
+      </c>
+      <c r="J27" s="6" t="s">
+        <v>831</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A28" s="6">
+        <v>27</v>
+      </c>
+      <c r="B28" s="6" t="s">
+        <v>427</v>
+      </c>
+      <c r="C28" s="28">
+        <v>44271</v>
+      </c>
+      <c r="D28" s="6">
+        <v>1</v>
+      </c>
+      <c r="E28" s="6">
+        <v>1</v>
+      </c>
+      <c r="F28" s="6">
+        <v>40</v>
+      </c>
+      <c r="G28" s="6" t="s">
+        <v>833</v>
+      </c>
+      <c r="H28" s="6" t="s">
+        <v>834</v>
+      </c>
+      <c r="I28" s="28">
+        <v>44271</v>
+      </c>
+      <c r="J28" s="6" t="s">
+        <v>831</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A29" s="6">
+        <v>28</v>
+      </c>
+      <c r="B29" s="6" t="s">
+        <v>430</v>
+      </c>
+      <c r="C29" s="28">
+        <v>44272</v>
+      </c>
+      <c r="D29" s="6">
+        <v>1</v>
+      </c>
+      <c r="E29" s="6">
+        <v>1</v>
+      </c>
+      <c r="F29" s="6">
+        <v>40</v>
+      </c>
+      <c r="G29" s="6" t="s">
+        <v>833</v>
+      </c>
+      <c r="H29" s="6" t="s">
+        <v>834</v>
+      </c>
+      <c r="I29" s="28">
+        <v>44272</v>
+      </c>
+      <c r="J29" s="6" t="s">
+        <v>831</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A30" s="6">
+        <v>29</v>
+      </c>
+      <c r="B30" s="6" t="s">
+        <v>433</v>
+      </c>
+      <c r="C30" s="28">
+        <v>44273</v>
+      </c>
+      <c r="D30" s="6">
+        <v>1</v>
+      </c>
+      <c r="E30" s="6">
+        <v>1</v>
+      </c>
+      <c r="F30" s="6">
+        <v>40</v>
+      </c>
+      <c r="G30" s="6" t="s">
+        <v>833</v>
+      </c>
+      <c r="H30" s="6" t="s">
+        <v>834</v>
+      </c>
+      <c r="I30" s="28">
+        <v>44273</v>
+      </c>
+      <c r="J30" s="6" t="s">
+        <v>831</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A31" s="6">
+        <v>30</v>
+      </c>
+      <c r="B31" s="6" t="s">
+        <v>436</v>
+      </c>
+      <c r="C31" s="28">
+        <v>44274</v>
+      </c>
+      <c r="D31" s="6">
+        <v>1</v>
+      </c>
+      <c r="E31" s="6">
+        <v>1</v>
+      </c>
+      <c r="F31" s="6">
+        <v>40</v>
+      </c>
+      <c r="G31" s="6" t="s">
+        <v>833</v>
+      </c>
+      <c r="H31" s="6" t="s">
+        <v>834</v>
+      </c>
+      <c r="I31" s="28">
+        <v>44274</v>
+      </c>
+      <c r="J31" s="6" t="s">
+        <v>831</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
add and fix: approval insert part
상신하는 기능 구현 1차 완료
</commit_message>
<xml_diff>
--- a/DB.xlsx
+++ b/DB.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2360" yWindow="560" windowWidth="16580" windowHeight="11000" tabRatio="919" activeTab="1"/>
+    <workbookView xWindow="2360" yWindow="560" windowWidth="16580" windowHeight="11000" tabRatio="919" firstSheet="16" activeTab="23"/>
   </bookViews>
   <sheets>
     <sheet name="member(sample)" sheetId="2" r:id="rId1"/>
@@ -69,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2896" uniqueCount="1200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2895" uniqueCount="1200">
   <si>
     <t xml:space="preserve">	서울특별시송파구올림픽로 99(잠실동, 잠실엘스)</t>
   </si>
@@ -18173,8 +18173,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G30"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
@@ -22564,8 +22564,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
@@ -23458,8 +23458,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
@@ -23602,9 +23602,7 @@
       <c r="D6" t="s">
         <v>1071</v>
       </c>
-      <c r="E6" s="42" t="s">
-        <v>1072</v>
-      </c>
+      <c r="E6" s="42"/>
       <c r="F6" s="43">
         <v>44197</v>
       </c>

</xml_diff>

<commit_message>
fix: sql컬럼추가 ! , 기타 approval수정
</commit_message>
<xml_diff>
--- a/DB.xlsx
+++ b/DB.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2780" yWindow="2240" windowWidth="19990" windowHeight="9940" tabRatio="919" firstSheet="10" activeTab="25"/>
+    <workbookView xWindow="2780" yWindow="2240" windowWidth="19990" windowHeight="9940" tabRatio="919" firstSheet="10" activeTab="27"/>
   </bookViews>
   <sheets>
     <sheet name="member(sample)" sheetId="2" r:id="rId1"/>
@@ -48,7 +48,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="20" hidden="1">JaeWook_ATTENDANCE!$A$1:$G$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="22" hidden="1">JaeWook_LEAVE!$A$1:$I$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'member(sample)'!$A$1:$Q$491</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="27" hidden="1">REFERENCE!$A$1:$C$49</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="27" hidden="1">REFERENCE!$A$1:$D$49</definedName>
     <definedName name="Apart" localSheetId="23">#REF!</definedName>
     <definedName name="Apart" localSheetId="24">#REF!</definedName>
     <definedName name="Apart">#REF!</definedName>
@@ -69,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2912" uniqueCount="1213">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2961" uniqueCount="1216">
   <si>
     <t xml:space="preserve">	서울특별시송파구올림픽로 99(잠실동, 잠실엘스)</t>
   </si>
@@ -4304,6 +4304,18 @@
   </si>
   <si>
     <t>appr_memo</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>READ</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>N</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>N</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -24807,8 +24819,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I65"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="Q30" sqref="Q30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
@@ -26986,15 +26998,15 @@
 
 <file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C49"/>
+  <dimension ref="A1:D49"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D34" sqref="D34"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>960</v>
       </c>
@@ -27004,8 +27016,11 @@
       <c r="C1" t="s">
         <v>962</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D1" t="s">
+        <v>1213</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A2">
         <v>1</v>
       </c>
@@ -27015,8 +27030,11 @@
       <c r="C2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D2" t="s">
+        <v>1214</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A3">
         <v>2</v>
       </c>
@@ -27026,8 +27044,11 @@
       <c r="C3">
         <v>17</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D3" t="s">
+        <v>1215</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A4">
         <v>3</v>
       </c>
@@ -27037,8 +27058,11 @@
       <c r="C4">
         <v>33</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D4" t="s">
+        <v>1214</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A5">
         <v>4</v>
       </c>
@@ -27048,8 +27072,11 @@
       <c r="C5">
         <v>2</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D5" t="s">
+        <v>1214</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A6">
         <v>5</v>
       </c>
@@ -27059,8 +27086,11 @@
       <c r="C6">
         <v>18</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D6" t="s">
+        <v>1215</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A7">
         <v>6</v>
       </c>
@@ -27070,8 +27100,11 @@
       <c r="C7">
         <v>34</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D7" t="s">
+        <v>1214</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A8">
         <v>7</v>
       </c>
@@ -27081,8 +27114,11 @@
       <c r="C8">
         <v>3</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D8" t="s">
+        <v>1214</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A9">
         <v>8</v>
       </c>
@@ -27092,8 +27128,11 @@
       <c r="C9">
         <v>19</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D9" t="s">
+        <v>1215</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A10">
         <v>9</v>
       </c>
@@ -27103,8 +27142,11 @@
       <c r="C10">
         <v>35</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D10" t="s">
+        <v>1214</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A11">
         <v>10</v>
       </c>
@@ -27114,8 +27156,11 @@
       <c r="C11">
         <v>4</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D11" t="s">
+        <v>1214</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A12">
         <v>11</v>
       </c>
@@ -27125,8 +27170,11 @@
       <c r="C12">
         <v>20</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D12" t="s">
+        <v>1215</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A13">
         <v>12</v>
       </c>
@@ -27136,8 +27184,11 @@
       <c r="C13">
         <v>36</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D13" t="s">
+        <v>1214</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A14">
         <v>13</v>
       </c>
@@ -27147,8 +27198,11 @@
       <c r="C14">
         <v>5</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D14" t="s">
+        <v>1214</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A15">
         <v>14</v>
       </c>
@@ -27158,8 +27212,11 @@
       <c r="C15">
         <v>21</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D15" t="s">
+        <v>1215</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A16">
         <v>15</v>
       </c>
@@ -27169,8 +27226,11 @@
       <c r="C16">
         <v>37</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D16" t="s">
+        <v>1214</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A17">
         <v>16</v>
       </c>
@@ -27180,8 +27240,11 @@
       <c r="C17">
         <v>6</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D17" t="s">
+        <v>1214</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A18">
         <v>17</v>
       </c>
@@ -27191,8 +27254,11 @@
       <c r="C18">
         <v>22</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D18" t="s">
+        <v>1215</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A19">
         <v>18</v>
       </c>
@@ -27202,8 +27268,11 @@
       <c r="C19">
         <v>38</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D19" t="s">
+        <v>1214</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A20">
         <v>19</v>
       </c>
@@ -27213,8 +27282,11 @@
       <c r="C20">
         <v>7</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D20" t="s">
+        <v>1214</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A21">
         <v>20</v>
       </c>
@@ -27224,8 +27296,11 @@
       <c r="C21">
         <v>23</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D21" t="s">
+        <v>1215</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A22">
         <v>21</v>
       </c>
@@ -27235,8 +27310,11 @@
       <c r="C22">
         <v>39</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D22" t="s">
+        <v>1214</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A23">
         <v>22</v>
       </c>
@@ -27246,8 +27324,11 @@
       <c r="C23">
         <v>8</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D23" t="s">
+        <v>1214</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A24">
         <v>23</v>
       </c>
@@ -27257,8 +27338,11 @@
       <c r="C24">
         <v>24</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D24" t="s">
+        <v>1215</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A25">
         <v>24</v>
       </c>
@@ -27268,8 +27352,11 @@
       <c r="C25">
         <v>1</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D25" t="s">
+        <v>1214</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A26">
         <v>25</v>
       </c>
@@ -27279,8 +27366,11 @@
       <c r="C26">
         <v>9</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D26" t="s">
+        <v>1214</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A27">
         <v>26</v>
       </c>
@@ -27290,8 +27380,11 @@
       <c r="C27">
         <v>25</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D27" t="s">
+        <v>1215</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A28">
         <v>27</v>
       </c>
@@ -27301,8 +27394,11 @@
       <c r="C28">
         <v>2</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D28" t="s">
+        <v>1214</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A29">
         <v>28</v>
       </c>
@@ -27312,8 +27408,11 @@
       <c r="C29">
         <v>10</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D29" t="s">
+        <v>1214</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A30">
         <v>29</v>
       </c>
@@ -27323,8 +27422,11 @@
       <c r="C30">
         <v>26</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D30" t="s">
+        <v>1215</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A31">
         <v>30</v>
       </c>
@@ -27334,8 +27436,11 @@
       <c r="C31">
         <v>3</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D31" t="s">
+        <v>1214</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A32">
         <v>31</v>
       </c>
@@ -27345,8 +27450,11 @@
       <c r="C32">
         <v>11</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D32" t="s">
+        <v>1214</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A33">
         <v>32</v>
       </c>
@@ -27356,8 +27464,11 @@
       <c r="C33">
         <v>27</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D33" t="s">
+        <v>1215</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A34">
         <v>33</v>
       </c>
@@ -27367,8 +27478,11 @@
       <c r="C34">
         <v>4</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D34" t="s">
+        <v>1214</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A35">
         <v>34</v>
       </c>
@@ -27378,8 +27492,11 @@
       <c r="C35">
         <v>12</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D35" t="s">
+        <v>1214</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A36">
         <v>35</v>
       </c>
@@ -27389,8 +27506,11 @@
       <c r="C36">
         <v>28</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D36" t="s">
+        <v>1215</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A37">
         <v>36</v>
       </c>
@@ -27400,8 +27520,11 @@
       <c r="C37">
         <v>5</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D37" t="s">
+        <v>1214</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A38">
         <v>37</v>
       </c>
@@ -27411,8 +27534,11 @@
       <c r="C38">
         <v>13</v>
       </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D38" t="s">
+        <v>1214</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A39">
         <v>38</v>
       </c>
@@ -27422,8 +27548,11 @@
       <c r="C39">
         <v>29</v>
       </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D39" t="s">
+        <v>1215</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A40">
         <v>39</v>
       </c>
@@ -27433,8 +27562,11 @@
       <c r="C40">
         <v>6</v>
       </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D40" t="s">
+        <v>1214</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A41">
         <v>40</v>
       </c>
@@ -27444,8 +27576,11 @@
       <c r="C41">
         <v>14</v>
       </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D41" t="s">
+        <v>1214</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A42">
         <v>41</v>
       </c>
@@ -27455,8 +27590,11 @@
       <c r="C42">
         <v>30</v>
       </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D42" t="s">
+        <v>1215</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A43">
         <v>42</v>
       </c>
@@ -27466,8 +27604,11 @@
       <c r="C43">
         <v>7</v>
       </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D43" t="s">
+        <v>1214</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A44">
         <v>43</v>
       </c>
@@ -27477,8 +27618,11 @@
       <c r="C44">
         <v>15</v>
       </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D44" t="s">
+        <v>1214</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A45">
         <v>44</v>
       </c>
@@ -27488,8 +27632,11 @@
       <c r="C45">
         <v>31</v>
       </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D45" t="s">
+        <v>1215</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A46">
         <v>45</v>
       </c>
@@ -27499,8 +27646,11 @@
       <c r="C46">
         <v>8</v>
       </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D46" t="s">
+        <v>1214</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A47">
         <v>46</v>
       </c>
@@ -27510,8 +27660,11 @@
       <c r="C47">
         <v>16</v>
       </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D47" t="s">
+        <v>1214</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A48">
         <v>47</v>
       </c>
@@ -27521,8 +27674,11 @@
       <c r="C48">
         <v>32</v>
       </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D48" t="s">
+        <v>1215</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A49">
         <v>48</v>
       </c>
@@ -27532,13 +27688,12 @@
       <c r="C49">
         <v>9</v>
       </c>
+      <c r="D49" t="s">
+        <v>1214</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:C49">
-    <sortState ref="A2:C49">
-      <sortCondition ref="B1:B49"/>
-    </sortState>
-  </autoFilter>
+  <autoFilter ref="A1:D49"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" r:id="rId1"/>

</xml_diff>

<commit_message>
fix: sampleData import 순서
</commit_message>
<xml_diff>
--- a/DB.xlsx
+++ b/DB.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="9900" yWindow="1620" windowWidth="17664" windowHeight="13680" tabRatio="919" activeTab="11"/>
+    <workbookView xWindow="9900" yWindow="1620" windowWidth="17664" windowHeight="13680" tabRatio="919" firstSheet="22" activeTab="27"/>
   </bookViews>
   <sheets>
     <sheet name="department" sheetId="5" r:id="rId1"/>
@@ -27,9 +27,9 @@
     <sheet name="Sunyoung_document" sheetId="30" r:id="rId13"/>
     <sheet name="Sunyoung_bizReport" sheetId="31" r:id="rId14"/>
     <sheet name="Sunyoung_note" sheetId="32" r:id="rId15"/>
-    <sheet name="Sunyoung_reservation" sheetId="42" r:id="rId16"/>
+    <sheet name="Sunyoung_re_category" sheetId="44" r:id="rId16"/>
     <sheet name="Sunyoung_resources" sheetId="43" r:id="rId17"/>
-    <sheet name="Sunyoung_re_category" sheetId="44" r:id="rId18"/>
+    <sheet name="Sunyoung_reservation" sheetId="42" r:id="rId18"/>
     <sheet name="SK_board" sheetId="16" r:id="rId19"/>
     <sheet name="SK_market" sheetId="17" r:id="rId20"/>
     <sheet name="SK_reply" sheetId="18" r:id="rId21"/>
@@ -37,26 +37,26 @@
     <sheet name="JaeWook_COMPANY" sheetId="20" r:id="rId23"/>
     <sheet name="JaeWook_ATTENDANCE" sheetId="21" r:id="rId24"/>
     <sheet name="JaeWook_ATT_BOARD" sheetId="22" r:id="rId25"/>
-    <sheet name="JaeWook_LEAVE" sheetId="23" r:id="rId26"/>
-    <sheet name="appr_form" sheetId="45" r:id="rId27"/>
-    <sheet name="approval" sheetId="39" r:id="rId28"/>
-    <sheet name="appr_accept" sheetId="40" r:id="rId29"/>
+    <sheet name="appr_form" sheetId="45" r:id="rId26"/>
+    <sheet name="approval" sheetId="39" r:id="rId27"/>
+    <sheet name="appr_accept" sheetId="40" r:id="rId28"/>
+    <sheet name="JaeWook_LEAVE" sheetId="23" r:id="rId29"/>
     <sheet name="REFERENCE" sheetId="41" r:id="rId30"/>
     <sheet name="mail_sender" sheetId="36" r:id="rId31"/>
     <sheet name="mail_receiver" sheetId="37" r:id="rId32"/>
     <sheet name="ma_attach" sheetId="38" r:id="rId33"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="28" hidden="1">appr_accept!$A$1:$I$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="27" hidden="1">approval!$A$1:$G$7</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="27" hidden="1">appr_accept!$A$1:$I$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="26" hidden="1">approval!$A$1:$G$7</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="24" hidden="1">JaeWook_ATT_BOARD!$A$1:$E$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="23" hidden="1">JaeWook_ATTENDANCE!$A$1:$G$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="25" hidden="1">JaeWook_LEAVE!$A$1:$I$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="28" hidden="1">JaeWook_LEAVE!$A$1:$I$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="31" hidden="1">mail_receiver!$A$1:$L$226</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="30" hidden="1">mail_sender!$A$1:$I$7</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'member(sample)'!$A$1:$S$491</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="29" hidden="1">REFERENCE!$A$1:$D$1</definedName>
-    <definedName name="Apart" localSheetId="27">#REF!</definedName>
+    <definedName name="Apart" localSheetId="26">#REF!</definedName>
     <definedName name="Apart" localSheetId="32">#REF!</definedName>
     <definedName name="Apart" localSheetId="31">#REF!</definedName>
     <definedName name="Apart" localSheetId="30">#REF!</definedName>
@@ -7942,7 +7942,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
@@ -10075,341 +10075,48 @@
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I11"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="Q26" sqref="Q26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="14.59765625" style="30" customWidth="1"/>
-    <col min="2" max="3" width="18.59765625" style="30" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="39" style="30" customWidth="1"/>
-    <col min="5" max="5" width="11.59765625" style="47" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.796875" style="47" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.59765625" style="47" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.296875" style="30" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.69921875" style="30" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19" style="30" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="43" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:2" s="43" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A1" s="42" t="s">
-        <v>1322</v>
+        <v>1355</v>
       </c>
       <c r="B1" s="42" t="s">
-        <v>1323</v>
-      </c>
-      <c r="C1" s="42" t="s">
-        <v>1324</v>
-      </c>
-      <c r="D1" s="42" t="s">
-        <v>1325</v>
-      </c>
-      <c r="E1" s="69" t="s">
-        <v>1326</v>
-      </c>
-      <c r="F1" s="69" t="s">
-        <v>1327</v>
-      </c>
-      <c r="G1" s="69" t="s">
-        <v>1328</v>
-      </c>
-      <c r="H1" s="42" t="s">
-        <v>1329</v>
-      </c>
-      <c r="I1" s="42" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.4">
+        <v>1360</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A2" s="65">
         <v>1</v>
       </c>
-      <c r="B2" s="65">
-        <v>1</v>
-      </c>
-      <c r="C2" s="65">
-        <v>1</v>
-      </c>
-      <c r="D2" s="65" t="s">
-        <v>1330</v>
-      </c>
-      <c r="E2" s="70" t="s">
-        <v>836</v>
-      </c>
-      <c r="F2" s="70" t="s">
-        <v>1331</v>
-      </c>
-      <c r="G2" s="70" t="s">
-        <v>1332</v>
-      </c>
-      <c r="H2" s="68">
-        <v>44409</v>
-      </c>
-      <c r="I2" s="65" t="s">
-        <v>356</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="B2" s="65" t="s">
+        <v>1359</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A3" s="65">
         <v>2</v>
       </c>
-      <c r="B3" s="65">
-        <v>2</v>
-      </c>
-      <c r="C3" s="65">
-        <v>2</v>
-      </c>
-      <c r="D3" s="65" t="s">
-        <v>1333</v>
-      </c>
-      <c r="E3" s="70" t="s">
-        <v>836</v>
-      </c>
-      <c r="F3" s="70" t="s">
-        <v>1334</v>
-      </c>
-      <c r="G3" s="70" t="s">
-        <v>1335</v>
-      </c>
-      <c r="H3" s="68">
-        <v>44410</v>
-      </c>
-      <c r="I3" s="65" t="s">
-        <v>356</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="B3" s="65" t="s">
+        <v>1358</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A4" s="65">
         <v>3</v>
       </c>
-      <c r="B4" s="65">
-        <v>3</v>
-      </c>
-      <c r="C4" s="65">
-        <v>3</v>
-      </c>
-      <c r="D4" s="65" t="s">
-        <v>1336</v>
-      </c>
-      <c r="E4" s="70" t="s">
-        <v>836</v>
-      </c>
-      <c r="F4" s="70" t="s">
-        <v>1337</v>
-      </c>
-      <c r="G4" s="70" t="s">
-        <v>1338</v>
-      </c>
-      <c r="H4" s="68">
-        <v>44411</v>
-      </c>
-      <c r="I4" s="65" t="s">
-        <v>356</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A5" s="65">
-        <v>4</v>
-      </c>
-      <c r="B5" s="65">
-        <v>1</v>
-      </c>
-      <c r="C5" s="65">
-        <v>4</v>
-      </c>
-      <c r="D5" s="65" t="s">
-        <v>1339</v>
-      </c>
-      <c r="E5" s="70" t="s">
-        <v>836</v>
-      </c>
-      <c r="F5" s="70" t="s">
-        <v>1335</v>
-      </c>
-      <c r="G5" s="70" t="s">
-        <v>1340</v>
-      </c>
-      <c r="H5" s="68">
-        <v>44412</v>
-      </c>
-      <c r="I5" s="65" t="s">
-        <v>356</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A6" s="65">
-        <v>5</v>
-      </c>
-      <c r="B6" s="65">
-        <v>2</v>
-      </c>
-      <c r="C6" s="65">
-        <v>5</v>
-      </c>
-      <c r="D6" s="65" t="s">
-        <v>1341</v>
-      </c>
-      <c r="E6" s="70" t="s">
-        <v>836</v>
-      </c>
-      <c r="F6" s="70" t="s">
-        <v>1335</v>
-      </c>
-      <c r="G6" s="70" t="s">
-        <v>1342</v>
-      </c>
-      <c r="H6" s="68">
-        <v>44413</v>
-      </c>
-      <c r="I6" s="65" t="s">
-        <v>356</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A7" s="65">
-        <v>6</v>
-      </c>
-      <c r="B7" s="65">
-        <v>1</v>
-      </c>
-      <c r="C7" s="65">
-        <v>6</v>
-      </c>
-      <c r="D7" s="65" t="s">
-        <v>1339</v>
-      </c>
-      <c r="E7" s="70" t="s">
-        <v>818</v>
-      </c>
-      <c r="F7" s="70" t="s">
-        <v>1337</v>
-      </c>
-      <c r="G7" s="70" t="s">
-        <v>1338</v>
-      </c>
-      <c r="H7" s="68">
-        <v>44414</v>
-      </c>
-      <c r="I7" s="65" t="s">
-        <v>356</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A8" s="65">
-        <v>7</v>
-      </c>
-      <c r="B8" s="65">
-        <v>2</v>
-      </c>
-      <c r="C8" s="65">
-        <v>7</v>
-      </c>
-      <c r="D8" s="65" t="s">
-        <v>1341</v>
-      </c>
-      <c r="E8" s="70" t="s">
-        <v>818</v>
-      </c>
-      <c r="F8" s="70" t="s">
-        <v>1334</v>
-      </c>
-      <c r="G8" s="70" t="s">
-        <v>1335</v>
-      </c>
-      <c r="H8" s="68">
-        <v>44415</v>
-      </c>
-      <c r="I8" s="65" t="s">
-        <v>356</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A9" s="65">
-        <v>8</v>
-      </c>
-      <c r="B9" s="65">
-        <v>1</v>
-      </c>
-      <c r="C9" s="65">
-        <v>8</v>
-      </c>
-      <c r="D9" s="65" t="s">
-        <v>1343</v>
-      </c>
-      <c r="E9" s="70" t="s">
-        <v>818</v>
-      </c>
-      <c r="F9" s="70" t="s">
-        <v>1331</v>
-      </c>
-      <c r="G9" s="70" t="s">
-        <v>1332</v>
-      </c>
-      <c r="H9" s="68">
-        <v>44416</v>
-      </c>
-      <c r="I9" s="65" t="s">
-        <v>356</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A10" s="65">
-        <v>9</v>
-      </c>
-      <c r="B10" s="65">
-        <v>2</v>
-      </c>
-      <c r="C10" s="65">
-        <v>9</v>
-      </c>
-      <c r="D10" s="65" t="s">
-        <v>1344</v>
-      </c>
-      <c r="E10" s="70" t="s">
-        <v>818</v>
-      </c>
-      <c r="F10" s="70" t="s">
-        <v>1335</v>
-      </c>
-      <c r="G10" s="70" t="s">
-        <v>1340</v>
-      </c>
-      <c r="H10" s="68">
-        <v>44417</v>
-      </c>
-      <c r="I10" s="65" t="s">
-        <v>356</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A11" s="65">
-        <v>10</v>
-      </c>
-      <c r="B11" s="65">
-        <v>3</v>
-      </c>
-      <c r="C11" s="65">
-        <v>10</v>
-      </c>
-      <c r="D11" s="65" t="s">
-        <v>1345</v>
-      </c>
-      <c r="E11" s="70" t="s">
-        <v>818</v>
-      </c>
-      <c r="F11" s="70" t="s">
-        <v>1335</v>
-      </c>
-      <c r="G11" s="70" t="s">
-        <v>1342</v>
-      </c>
-      <c r="H11" s="68">
-        <v>44418</v>
-      </c>
-      <c r="I11" s="65" t="s">
-        <v>356</v>
+      <c r="B4" s="65" t="s">
+        <v>1357</v>
       </c>
     </row>
   </sheetData>
@@ -10553,48 +10260,341 @@
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="14.59765625" style="30" customWidth="1"/>
-    <col min="2" max="2" width="19" style="30" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="18.59765625" style="30" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="39" style="30" customWidth="1"/>
+    <col min="5" max="5" width="11.59765625" style="47" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.796875" style="47" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.59765625" style="47" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.296875" style="30" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.69921875" style="30" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="43" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:9" s="43" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A1" s="42" t="s">
-        <v>1355</v>
+        <v>1322</v>
       </c>
       <c r="B1" s="42" t="s">
-        <v>1360</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.4">
+        <v>1323</v>
+      </c>
+      <c r="C1" s="42" t="s">
+        <v>1324</v>
+      </c>
+      <c r="D1" s="42" t="s">
+        <v>1325</v>
+      </c>
+      <c r="E1" s="69" t="s">
+        <v>1326</v>
+      </c>
+      <c r="F1" s="69" t="s">
+        <v>1327</v>
+      </c>
+      <c r="G1" s="69" t="s">
+        <v>1328</v>
+      </c>
+      <c r="H1" s="42" t="s">
+        <v>1329</v>
+      </c>
+      <c r="I1" s="42" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A2" s="65">
         <v>1</v>
       </c>
-      <c r="B2" s="65" t="s">
-        <v>1359</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="B2" s="65">
+        <v>1</v>
+      </c>
+      <c r="C2" s="65">
+        <v>1</v>
+      </c>
+      <c r="D2" s="65" t="s">
+        <v>1330</v>
+      </c>
+      <c r="E2" s="70" t="s">
+        <v>836</v>
+      </c>
+      <c r="F2" s="70" t="s">
+        <v>1331</v>
+      </c>
+      <c r="G2" s="70" t="s">
+        <v>1332</v>
+      </c>
+      <c r="H2" s="68">
+        <v>44409</v>
+      </c>
+      <c r="I2" s="65" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A3" s="65">
         <v>2</v>
       </c>
-      <c r="B3" s="65" t="s">
-        <v>1358</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="B3" s="65">
+        <v>2</v>
+      </c>
+      <c r="C3" s="65">
+        <v>2</v>
+      </c>
+      <c r="D3" s="65" t="s">
+        <v>1333</v>
+      </c>
+      <c r="E3" s="70" t="s">
+        <v>836</v>
+      </c>
+      <c r="F3" s="70" t="s">
+        <v>1334</v>
+      </c>
+      <c r="G3" s="70" t="s">
+        <v>1335</v>
+      </c>
+      <c r="H3" s="68">
+        <v>44410</v>
+      </c>
+      <c r="I3" s="65" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A4" s="65">
         <v>3</v>
       </c>
-      <c r="B4" s="65" t="s">
-        <v>1357</v>
+      <c r="B4" s="65">
+        <v>3</v>
+      </c>
+      <c r="C4" s="65">
+        <v>3</v>
+      </c>
+      <c r="D4" s="65" t="s">
+        <v>1336</v>
+      </c>
+      <c r="E4" s="70" t="s">
+        <v>836</v>
+      </c>
+      <c r="F4" s="70" t="s">
+        <v>1337</v>
+      </c>
+      <c r="G4" s="70" t="s">
+        <v>1338</v>
+      </c>
+      <c r="H4" s="68">
+        <v>44411</v>
+      </c>
+      <c r="I4" s="65" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A5" s="65">
+        <v>4</v>
+      </c>
+      <c r="B5" s="65">
+        <v>1</v>
+      </c>
+      <c r="C5" s="65">
+        <v>4</v>
+      </c>
+      <c r="D5" s="65" t="s">
+        <v>1339</v>
+      </c>
+      <c r="E5" s="70" t="s">
+        <v>836</v>
+      </c>
+      <c r="F5" s="70" t="s">
+        <v>1335</v>
+      </c>
+      <c r="G5" s="70" t="s">
+        <v>1340</v>
+      </c>
+      <c r="H5" s="68">
+        <v>44412</v>
+      </c>
+      <c r="I5" s="65" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A6" s="65">
+        <v>5</v>
+      </c>
+      <c r="B6" s="65">
+        <v>2</v>
+      </c>
+      <c r="C6" s="65">
+        <v>5</v>
+      </c>
+      <c r="D6" s="65" t="s">
+        <v>1341</v>
+      </c>
+      <c r="E6" s="70" t="s">
+        <v>836</v>
+      </c>
+      <c r="F6" s="70" t="s">
+        <v>1335</v>
+      </c>
+      <c r="G6" s="70" t="s">
+        <v>1342</v>
+      </c>
+      <c r="H6" s="68">
+        <v>44413</v>
+      </c>
+      <c r="I6" s="65" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A7" s="65">
+        <v>6</v>
+      </c>
+      <c r="B7" s="65">
+        <v>1</v>
+      </c>
+      <c r="C7" s="65">
+        <v>6</v>
+      </c>
+      <c r="D7" s="65" t="s">
+        <v>1339</v>
+      </c>
+      <c r="E7" s="70" t="s">
+        <v>818</v>
+      </c>
+      <c r="F7" s="70" t="s">
+        <v>1337</v>
+      </c>
+      <c r="G7" s="70" t="s">
+        <v>1338</v>
+      </c>
+      <c r="H7" s="68">
+        <v>44414</v>
+      </c>
+      <c r="I7" s="65" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A8" s="65">
+        <v>7</v>
+      </c>
+      <c r="B8" s="65">
+        <v>2</v>
+      </c>
+      <c r="C8" s="65">
+        <v>7</v>
+      </c>
+      <c r="D8" s="65" t="s">
+        <v>1341</v>
+      </c>
+      <c r="E8" s="70" t="s">
+        <v>818</v>
+      </c>
+      <c r="F8" s="70" t="s">
+        <v>1334</v>
+      </c>
+      <c r="G8" s="70" t="s">
+        <v>1335</v>
+      </c>
+      <c r="H8" s="68">
+        <v>44415</v>
+      </c>
+      <c r="I8" s="65" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A9" s="65">
+        <v>8</v>
+      </c>
+      <c r="B9" s="65">
+        <v>1</v>
+      </c>
+      <c r="C9" s="65">
+        <v>8</v>
+      </c>
+      <c r="D9" s="65" t="s">
+        <v>1343</v>
+      </c>
+      <c r="E9" s="70" t="s">
+        <v>818</v>
+      </c>
+      <c r="F9" s="70" t="s">
+        <v>1331</v>
+      </c>
+      <c r="G9" s="70" t="s">
+        <v>1332</v>
+      </c>
+      <c r="H9" s="68">
+        <v>44416</v>
+      </c>
+      <c r="I9" s="65" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A10" s="65">
+        <v>9</v>
+      </c>
+      <c r="B10" s="65">
+        <v>2</v>
+      </c>
+      <c r="C10" s="65">
+        <v>9</v>
+      </c>
+      <c r="D10" s="65" t="s">
+        <v>1344</v>
+      </c>
+      <c r="E10" s="70" t="s">
+        <v>818</v>
+      </c>
+      <c r="F10" s="70" t="s">
+        <v>1335</v>
+      </c>
+      <c r="G10" s="70" t="s">
+        <v>1340</v>
+      </c>
+      <c r="H10" s="68">
+        <v>44417</v>
+      </c>
+      <c r="I10" s="65" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A11" s="65">
+        <v>10</v>
+      </c>
+      <c r="B11" s="65">
+        <v>3</v>
+      </c>
+      <c r="C11" s="65">
+        <v>10</v>
+      </c>
+      <c r="D11" s="65" t="s">
+        <v>1345</v>
+      </c>
+      <c r="E11" s="70" t="s">
+        <v>818</v>
+      </c>
+      <c r="F11" s="70" t="s">
+        <v>1335</v>
+      </c>
+      <c r="G11" s="70" t="s">
+        <v>1342</v>
+      </c>
+      <c r="H11" s="68">
+        <v>44418</v>
+      </c>
+      <c r="I11" s="65" t="s">
+        <v>356</v>
       </c>
     </row>
   </sheetData>
@@ -28293,267 +28293,6 @@
 
 <file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I8"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
-  <cols>
-    <col min="1" max="1" width="14.09765625" customWidth="1"/>
-    <col min="2" max="2" width="9.5" customWidth="1"/>
-    <col min="3" max="3" width="15.796875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.09765625" customWidth="1"/>
-    <col min="6" max="6" width="13.296875" customWidth="1"/>
-    <col min="7" max="7" width="15.796875" customWidth="1"/>
-    <col min="8" max="8" width="18.59765625" customWidth="1"/>
-    <col min="9" max="9" width="14.09765625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:9" s="30" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="56" t="s">
-        <v>711</v>
-      </c>
-      <c r="B1" s="56" t="s">
-        <v>383</v>
-      </c>
-      <c r="C1" s="56" t="s">
-        <v>1237</v>
-      </c>
-      <c r="D1" s="56" t="s">
-        <v>404</v>
-      </c>
-      <c r="E1" s="56" t="s">
-        <v>1238</v>
-      </c>
-      <c r="F1" s="56" t="s">
-        <v>1239</v>
-      </c>
-      <c r="G1" s="56" t="s">
-        <v>1240</v>
-      </c>
-      <c r="H1" s="56" t="s">
-        <v>1241</v>
-      </c>
-      <c r="I1" s="56" t="s">
-        <v>1242</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" s="30" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="54">
-        <v>1</v>
-      </c>
-      <c r="B2" s="54">
-        <v>2</v>
-      </c>
-      <c r="C2" s="57">
-        <v>44242</v>
-      </c>
-      <c r="D2" s="57">
-        <v>44249</v>
-      </c>
-      <c r="E2" s="56">
-        <v>6</v>
-      </c>
-      <c r="F2" s="56" t="s">
-        <v>1243</v>
-      </c>
-      <c r="G2" s="56" t="s">
-        <v>1244</v>
-      </c>
-      <c r="H2" s="57">
-        <v>44232</v>
-      </c>
-      <c r="I2" s="58" t="s">
-        <v>1245</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" s="30" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="54">
-        <v>2</v>
-      </c>
-      <c r="B3" s="54">
-        <v>3</v>
-      </c>
-      <c r="C3" s="57">
-        <v>44299</v>
-      </c>
-      <c r="D3" s="57">
-        <v>44301</v>
-      </c>
-      <c r="E3" s="56">
-        <v>3</v>
-      </c>
-      <c r="F3" s="56" t="s">
-        <v>1243</v>
-      </c>
-      <c r="G3" s="56" t="s">
-        <v>1246</v>
-      </c>
-      <c r="H3" s="57">
-        <v>44296</v>
-      </c>
-      <c r="I3" s="58" t="s">
-        <v>1245</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" s="30" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="54">
-        <v>3</v>
-      </c>
-      <c r="B4" s="54">
-        <v>4</v>
-      </c>
-      <c r="C4" s="57">
-        <v>44361</v>
-      </c>
-      <c r="D4" s="57">
-        <v>44365</v>
-      </c>
-      <c r="E4" s="56">
-        <v>5</v>
-      </c>
-      <c r="F4" s="56" t="s">
-        <v>1243</v>
-      </c>
-      <c r="G4" s="56" t="s">
-        <v>1247</v>
-      </c>
-      <c r="H4" s="57">
-        <v>44348</v>
-      </c>
-      <c r="I4" s="58" t="s">
-        <v>1245</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A5" s="54">
-        <v>4</v>
-      </c>
-      <c r="B5" s="54">
-        <v>5</v>
-      </c>
-      <c r="C5" s="57">
-        <v>44369</v>
-      </c>
-      <c r="D5" s="57">
-        <v>44370</v>
-      </c>
-      <c r="E5" s="56">
-        <v>2</v>
-      </c>
-      <c r="F5" s="56" t="s">
-        <v>1243</v>
-      </c>
-      <c r="G5" s="56" t="s">
-        <v>1248</v>
-      </c>
-      <c r="H5" s="57">
-        <v>44368</v>
-      </c>
-      <c r="I5" s="58" t="s">
-        <v>1245</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A6" s="59">
-        <v>17</v>
-      </c>
-      <c r="B6" s="59">
-        <v>1</v>
-      </c>
-      <c r="C6" s="60">
-        <v>44383</v>
-      </c>
-      <c r="D6" s="60">
-        <v>44385</v>
-      </c>
-      <c r="E6" s="58">
-        <v>3</v>
-      </c>
-      <c r="F6" s="58" t="s">
-        <v>1249</v>
-      </c>
-      <c r="G6" s="58" t="s">
-        <v>1250</v>
-      </c>
-      <c r="H6" s="61">
-        <v>44385</v>
-      </c>
-      <c r="I6" s="58" t="s">
-        <v>1251</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A7" s="59">
-        <v>25</v>
-      </c>
-      <c r="B7" s="59">
-        <v>1</v>
-      </c>
-      <c r="C7" s="60">
-        <v>44393</v>
-      </c>
-      <c r="D7" s="60">
-        <v>44393</v>
-      </c>
-      <c r="E7" s="58">
-        <v>1</v>
-      </c>
-      <c r="F7" s="58" t="s">
-        <v>1252</v>
-      </c>
-      <c r="G7" s="58" t="s">
-        <v>1253</v>
-      </c>
-      <c r="H7" s="61">
-        <v>44391</v>
-      </c>
-      <c r="I7" s="58" t="s">
-        <v>1245</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A8" s="59">
-        <v>27</v>
-      </c>
-      <c r="B8" s="59">
-        <v>1</v>
-      </c>
-      <c r="C8" s="60">
-        <v>44405</v>
-      </c>
-      <c r="D8" s="60">
-        <v>44407</v>
-      </c>
-      <c r="E8" s="58">
-        <v>2</v>
-      </c>
-      <c r="F8" s="58" t="s">
-        <v>1249</v>
-      </c>
-      <c r="G8" s="58" t="s">
-        <v>1250</v>
-      </c>
-      <c r="H8" s="61">
-        <v>44405</v>
-      </c>
-      <c r="I8" s="58" t="s">
-        <v>1251</v>
-      </c>
-    </row>
-  </sheetData>
-  <autoFilter ref="A1:I1"/>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -28861,7 +28600,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G18"/>
   <sheetViews>
@@ -29149,12 +28888,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K19" sqref="K19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -29707,6 +29446,267 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I8"/>
+  <sheetViews>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="1" max="1" width="14.09765625" customWidth="1"/>
+    <col min="2" max="2" width="9.5" customWidth="1"/>
+    <col min="3" max="3" width="15.796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.09765625" customWidth="1"/>
+    <col min="6" max="6" width="13.296875" customWidth="1"/>
+    <col min="7" max="7" width="15.796875" customWidth="1"/>
+    <col min="8" max="8" width="18.59765625" customWidth="1"/>
+    <col min="9" max="9" width="14.09765625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" s="30" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="56" t="s">
+        <v>711</v>
+      </c>
+      <c r="B1" s="56" t="s">
+        <v>383</v>
+      </c>
+      <c r="C1" s="56" t="s">
+        <v>1237</v>
+      </c>
+      <c r="D1" s="56" t="s">
+        <v>404</v>
+      </c>
+      <c r="E1" s="56" t="s">
+        <v>1238</v>
+      </c>
+      <c r="F1" s="56" t="s">
+        <v>1239</v>
+      </c>
+      <c r="G1" s="56" t="s">
+        <v>1240</v>
+      </c>
+      <c r="H1" s="56" t="s">
+        <v>1241</v>
+      </c>
+      <c r="I1" s="56" t="s">
+        <v>1242</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" s="30" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A2" s="54">
+        <v>1</v>
+      </c>
+      <c r="B2" s="54">
+        <v>2</v>
+      </c>
+      <c r="C2" s="57">
+        <v>44242</v>
+      </c>
+      <c r="D2" s="57">
+        <v>44249</v>
+      </c>
+      <c r="E2" s="56">
+        <v>6</v>
+      </c>
+      <c r="F2" s="56" t="s">
+        <v>1243</v>
+      </c>
+      <c r="G2" s="56" t="s">
+        <v>1244</v>
+      </c>
+      <c r="H2" s="57">
+        <v>44232</v>
+      </c>
+      <c r="I2" s="58" t="s">
+        <v>1245</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" s="30" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A3" s="54">
+        <v>2</v>
+      </c>
+      <c r="B3" s="54">
+        <v>3</v>
+      </c>
+      <c r="C3" s="57">
+        <v>44299</v>
+      </c>
+      <c r="D3" s="57">
+        <v>44301</v>
+      </c>
+      <c r="E3" s="56">
+        <v>3</v>
+      </c>
+      <c r="F3" s="56" t="s">
+        <v>1243</v>
+      </c>
+      <c r="G3" s="56" t="s">
+        <v>1246</v>
+      </c>
+      <c r="H3" s="57">
+        <v>44296</v>
+      </c>
+      <c r="I3" s="58" t="s">
+        <v>1245</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" s="30" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A4" s="54">
+        <v>3</v>
+      </c>
+      <c r="B4" s="54">
+        <v>4</v>
+      </c>
+      <c r="C4" s="57">
+        <v>44361</v>
+      </c>
+      <c r="D4" s="57">
+        <v>44365</v>
+      </c>
+      <c r="E4" s="56">
+        <v>5</v>
+      </c>
+      <c r="F4" s="56" t="s">
+        <v>1243</v>
+      </c>
+      <c r="G4" s="56" t="s">
+        <v>1247</v>
+      </c>
+      <c r="H4" s="57">
+        <v>44348</v>
+      </c>
+      <c r="I4" s="58" t="s">
+        <v>1245</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A5" s="54">
+        <v>4</v>
+      </c>
+      <c r="B5" s="54">
+        <v>5</v>
+      </c>
+      <c r="C5" s="57">
+        <v>44369</v>
+      </c>
+      <c r="D5" s="57">
+        <v>44370</v>
+      </c>
+      <c r="E5" s="56">
+        <v>2</v>
+      </c>
+      <c r="F5" s="56" t="s">
+        <v>1243</v>
+      </c>
+      <c r="G5" s="56" t="s">
+        <v>1248</v>
+      </c>
+      <c r="H5" s="57">
+        <v>44368</v>
+      </c>
+      <c r="I5" s="58" t="s">
+        <v>1245</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A6" s="59">
+        <v>17</v>
+      </c>
+      <c r="B6" s="59">
+        <v>1</v>
+      </c>
+      <c r="C6" s="60">
+        <v>44383</v>
+      </c>
+      <c r="D6" s="60">
+        <v>44385</v>
+      </c>
+      <c r="E6" s="58">
+        <v>3</v>
+      </c>
+      <c r="F6" s="58" t="s">
+        <v>1249</v>
+      </c>
+      <c r="G6" s="58" t="s">
+        <v>1250</v>
+      </c>
+      <c r="H6" s="61">
+        <v>44385</v>
+      </c>
+      <c r="I6" s="58" t="s">
+        <v>1251</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A7" s="59">
+        <v>25</v>
+      </c>
+      <c r="B7" s="59">
+        <v>1</v>
+      </c>
+      <c r="C7" s="60">
+        <v>44393</v>
+      </c>
+      <c r="D7" s="60">
+        <v>44393</v>
+      </c>
+      <c r="E7" s="58">
+        <v>1</v>
+      </c>
+      <c r="F7" s="58" t="s">
+        <v>1252</v>
+      </c>
+      <c r="G7" s="58" t="s">
+        <v>1253</v>
+      </c>
+      <c r="H7" s="61">
+        <v>44391</v>
+      </c>
+      <c r="I7" s="58" t="s">
+        <v>1245</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A8" s="59">
+        <v>27</v>
+      </c>
+      <c r="B8" s="59">
+        <v>1</v>
+      </c>
+      <c r="C8" s="60">
+        <v>44405</v>
+      </c>
+      <c r="D8" s="60">
+        <v>44407</v>
+      </c>
+      <c r="E8" s="58">
+        <v>2</v>
+      </c>
+      <c r="F8" s="58" t="s">
+        <v>1249</v>
+      </c>
+      <c r="G8" s="58" t="s">
+        <v>1250</v>
+      </c>
+      <c r="H8" s="61">
+        <v>44405</v>
+      </c>
+      <c r="I8" s="58" t="s">
+        <v>1251</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:I1"/>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>